<commit_message>
Updated list of radiocarbon dates
</commit_message>
<xml_diff>
--- a/List_Radiocarbon_Dates.xlsx
+++ b/List_Radiocarbon_Dates.xlsx
@@ -506,12 +506,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -520,16 +529,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -815,1019 +824,1019 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="4" customWidth="1"/>
-    <col min="4" max="4" width="55.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.44140625" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="11.5546875" style="3"/>
+    <col min="1" max="1" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="2" customWidth="1"/>
+    <col min="4" max="4" width="55.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.44140625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>23</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>30</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>34</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>24</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="1">
         <v>20</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="1">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="1">
         <v>30</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="1">
         <v>9</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="1">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="1">
         <v>23</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="1">
         <v>7</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="1">
         <v>30</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="1">
         <v>4</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="1">
         <v>3</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="1">
         <v>7</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="1">
         <v>8</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="2" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="1">
         <v>14</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="2" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="1">
         <v>9</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="1">
         <v>49</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="1">
         <v>22</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="1">
         <v>14</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="1">
         <v>4</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="1">
         <v>5</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="1">
         <v>30</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="1">
         <v>7</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="1">
         <v>5</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="1">
         <v>10</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="1">
         <v>9</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="1">
         <v>8</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="1">
         <v>10</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="1">
         <v>3</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="1">
         <v>4</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="1">
         <v>4</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="C40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="1">
         <v>15</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="1">
         <v>11</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="1">
         <v>14</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="2" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="1">
         <v>4</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="C44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="1">
         <v>6</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" s="4" t="s">
+      <c r="C45" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="1">
         <v>11</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="C46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="1">
         <v>10</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="4" t="s">
+      <c r="C47" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="1">
         <v>6</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="4" t="s">
+      <c r="C48" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="1">
         <v>14</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="4" t="s">
+      <c r="C49" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="1">
         <v>13</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="4" t="s">
+      <c r="C50" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="1">
         <v>11</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="4" t="s">
+      <c r="C51" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="1">
         <v>4</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" s="4" t="s">
+      <c r="C52" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="1">
         <v>3</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="1">
         <v>17</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="1">
         <v>4</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="1">
         <v>20</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="4" t="s">
+      <c r="C56" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="1">
         <v>18</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" s="4" t="s">
+      <c r="C57" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="1">
         <v>15</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D58" s="4" t="s">
+      <c r="C58" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="1">
         <v>16</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="2" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update April 21, 2020
</commit_message>
<xml_diff>
--- a/List_Radiocarbon_Dates.xlsx
+++ b/List_Radiocarbon_Dates.xlsx
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated list for publication
</commit_message>
<xml_diff>
--- a/List_Radiocarbon_Dates.xlsx
+++ b/List_Radiocarbon_Dates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="145">
   <si>
     <t>CoreID</t>
   </si>
@@ -218,21 +218,12 @@
     <t>Unpublished</t>
   </si>
   <si>
-    <t>Personal communication: Ulrike.Herzschuh@awi.de</t>
-  </si>
-  <si>
     <t>EN18208.csv</t>
   </si>
   <si>
     <t>PG2201.csv</t>
   </si>
   <si>
-    <t>Personal communication: Stuart.Vyse@awi.de</t>
-  </si>
-  <si>
-    <t>Personal communication: Boris.Biskaborn@awi.de</t>
-  </si>
-  <si>
     <t>20190415_Biskaborn_Beti_und_Bouchard-2.xlsx</t>
   </si>
   <si>
@@ -318,9 +309,6 @@
   </si>
   <si>
     <t>Publication \\\ Unpublished</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.quascirev.2010.04.024 \\\ Personal communication: Luise.Schulte@awi.de</t>
   </si>
   <si>
     <t>Radiocarbon Dating Overview_6.xlsx \\\ 
@@ -332,149 +320,158 @@
 Radiocarbon Dating Overview_6.xlsx</t>
   </si>
   <si>
+    <t>Pangaea \\\ Unpublished</t>
+  </si>
+  <si>
+    <t>PG1756_14C-ages.tab</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.708169</t>
+  </si>
+  <si>
+    <t>Siberia_pollen_dating_data.tab</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.909360</t>
+  </si>
+  <si>
+    <t>PG1200_14C_ages.tab</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.385641</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.385642</t>
+  </si>
+  <si>
+    <t>PG1204_14C_ages.tab</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.385643</t>
+  </si>
+  <si>
+    <t>PG1205_14C_ages.tab</t>
+  </si>
+  <si>
+    <t>PG1212_14C_ages.tab</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.385644</t>
+  </si>
+  <si>
+    <t>PG1214_14C_ages.tab</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.385645</t>
+  </si>
+  <si>
+    <t>PG1227_age_determination.tab</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.56565</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1046/j.1365-246X.2002.01625.x</t>
+  </si>
+  <si>
+    <t>150-1-109.pdf</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.128662</t>
+  </si>
+  <si>
+    <t>PG1440_LakeNikolai_sedimentology.tab</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10933-012-9580-y</t>
+  </si>
+  <si>
+    <t>Hoff2012_Article_LateHoloceneDiatomAssemblagesI.pdf</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.gloplacha.2015.07.010</t>
+  </si>
+  <si>
+    <t>1-s2.0-S0921818115001563-main.pdf</t>
+  </si>
+  <si>
+    <t>PG1967_age_det.tab</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.855417</t>
+  </si>
+  <si>
+    <t>PG1972-1_age_det.tab</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.780526</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.780385</t>
+  </si>
+  <si>
+    <t>PG1975-1_age_det.tab</t>
+  </si>
+  <si>
+    <t>PG1984_age_det.tab \\\
+Alle_C14-Daten_BorisB.xlsx</t>
+  </si>
+  <si>
+    <t>1-s2.0-S0277379110001332-main.pdf \\\ 
+20180524_Schulte.xlsx</t>
+  </si>
+  <si>
+    <t>PG2022-1_age_det.tab \\\
+Radiocarbon Dating Overview_6.xlsx</t>
+  </si>
+  <si>
+    <t>PG2023-2_age_det.tab \\\
+Radiocarbon Dating Overview_6.xlsx</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s41063-016-0025-0</t>
+  </si>
+  <si>
+    <t>Publication \\\ Supplementary material</t>
+  </si>
+  <si>
+    <t>Lenz2016_Article_ImpactsOfShoreExpansionAndCatc.pdf</t>
+  </si>
+  <si>
+    <t>Lenz2016_Article_ImpactsOfShoreExpansionAndCatc.pdf \\\
+41063_2016_25_MOESM4_ESM.pdf</t>
+  </si>
+  <si>
+    <t>Tel2006_14C-dating.tab</t>
+  </si>
+  <si>
+    <t>https://doi.pangaea.de/10.1594/PANGAEA.914417</t>
+  </si>
+  <si>
+    <t>Working group: "High-latitude Biodiversity" https://www.awi.de/en/science/geosciences/polar-terrestrial-environmental-systems/research-foci/high-latitude-biodiversity.html; Personal communication: Kathleen.Stoof-Leichsenring@awi.de</t>
+  </si>
+  <si>
     <t>https://doi.pangaea.de/10.1594/PANGAEA.842564 \\\
 https://doi.pangaea.de/10.1594/PANGAEA.842563 \\\
-Personal communication: Ulrike.Herzschuh@awi.de</t>
-  </si>
-  <si>
-    <t>Pangaea \\\ Unpublished</t>
-  </si>
-  <si>
-    <t>PG1756_14C-ages.tab</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.708169</t>
-  </si>
-  <si>
-    <t>Siberia_pollen_dating_data.tab</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.909360</t>
-  </si>
-  <si>
-    <t>PG1200_14C_ages.tab</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.385641</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.385642</t>
-  </si>
-  <si>
-    <t>PG1204_14C_ages.tab</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.385643</t>
-  </si>
-  <si>
-    <t>PG1205_14C_ages.tab</t>
-  </si>
-  <si>
-    <t>PG1212_14C_ages.tab</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.385644</t>
-  </si>
-  <si>
-    <t>PG1214_14C_ages.tab</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.385645</t>
-  </si>
-  <si>
-    <t>PG1227_age_determination.tab</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.56565</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1046/j.1365-246X.2002.01625.x</t>
-  </si>
-  <si>
-    <t>150-1-109.pdf</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.128662</t>
-  </si>
-  <si>
-    <t>PG1440_LakeNikolai_sedimentology.tab</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/s10933-012-9580-y</t>
-  </si>
-  <si>
-    <t>Hoff2012_Article_LateHoloceneDiatomAssemblagesI.pdf</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.gloplacha.2015.07.010</t>
-  </si>
-  <si>
-    <t>1-s2.0-S0921818115001563-main.pdf</t>
-  </si>
-  <si>
-    <t>PG1967_age_det.tab</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.855417</t>
-  </si>
-  <si>
-    <t>PG1972-1_age_det.tab</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.780526</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.780385</t>
-  </si>
-  <si>
-    <t>PG1975-1_age_det.tab</t>
-  </si>
-  <si>
-    <t>PG1984_age_det.tab \\\
-Alle_C14-Daten_BorisB.xlsx</t>
+Working group: "High-latitude Biodiversity" https://www.awi.de/en/science/geosciences/polar-terrestrial-environmental-systems/research-foci/high-latitude-biodiversity.html; Personal communication: Kathleen.Stoof-Leichsenring@awi.de</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.quascirev.2010.04.024 \\\ Working group: "High-latitude Biodiversity" https://www.awi.de/en/science/geosciences/polar-terrestrial-environmental-systems/research-foci/high-latitude-biodiversity.html; Personal communication: Kathleen.Stoof-Leichsenring@awi.de</t>
+  </si>
+  <si>
+    <t>Working group: "Arctic Lake System Dynamics" https://www.awi.de/en/science/geosciences/polar-terrestrial-environmental-systems/research-foci/arctic-lake-system-dynamics.html; Personal communication: Boris.Biskaborn@awi.de</t>
   </si>
   <si>
     <t>https://doi.pangaea.de/10.1594/PANGAEA.776407 \\\
-Personal communication: Boris.Biskaborn@awi.de</t>
-  </si>
-  <si>
-    <t>1-s2.0-S0277379110001332-main.pdf \\\ 
-20180524_Schulte.xlsx</t>
-  </si>
-  <si>
-    <t>PG2022-1_age_det.tab \\\
-Radiocarbon Dating Overview_6.xlsx</t>
+Working group: "Arctic Lake System Dynamics" https://www.awi.de/en/science/geosciences/polar-terrestrial-environmental-systems/research-foci/arctic-lake-system-dynamics.html; Personal communication: Boris.Biskaborn@awi.de</t>
   </si>
   <si>
     <t>https://doi.pangaea.de/10.1594/PANGAEA.848894 \\\
-Personal communication: Boris.Biskaborn@awi.de</t>
-  </si>
-  <si>
-    <t>PG2023-2_age_det.tab \\\
-Radiocarbon Dating Overview_6.xlsx</t>
+Working group: "Arctic Lake System Dynamics" https://www.awi.de/en/science/geosciences/polar-terrestrial-environmental-systems/research-foci/arctic-lake-system-dynamics.html; Personal communication: Boris.Biskaborn@awi.de</t>
   </si>
   <si>
     <t>https://doi.pangaea.de/10.1594/PANGAEA.848897 \\\
-Personal communication: Boris.Biskaborn@awi.de</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1007/s41063-016-0025-0</t>
-  </si>
-  <si>
-    <t>Publication \\\ Supplementary material</t>
-  </si>
-  <si>
-    <t>Lenz2016_Article_ImpactsOfShoreExpansionAndCatc.pdf</t>
-  </si>
-  <si>
-    <t>Lenz2016_Article_ImpactsOfShoreExpansionAndCatc.pdf \\\
-41063_2016_25_MOESM4_ESM.pdf</t>
-  </si>
-  <si>
-    <t>Tel2006_14C-dating.tab</t>
-  </si>
-  <si>
-    <t>https://doi.pangaea.de/10.1594/PANGAEA.914417</t>
+Working group: "Arctic Lake System Dynamics" https://www.awi.de/en/science/geosciences/polar-terrestrial-environmental-systems/research-foci/arctic-lake-system-dynamics.html; Personal communication: Boris.Biskaborn@awi.de</t>
   </si>
 </sst>
 </file>
@@ -823,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:E43"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,7 +830,7 @@
     <col min="2" max="2" width="15.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" customWidth="1"/>
     <col min="4" max="4" width="55.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" style="2" customWidth="1"/>
     <col min="6" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
@@ -854,7 +851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -865,13 +862,13 @@
         <v>63</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -882,13 +879,13 @@
         <v>63</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -899,13 +896,13 @@
         <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -913,16 +910,16 @@
         <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -933,13 +930,13 @@
         <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -950,13 +947,13 @@
         <v>63</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -967,13 +964,13 @@
         <v>63</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -984,13 +981,13 @@
         <v>63</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1001,10 +998,10 @@
         <v>63</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>64</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1015,13 +1012,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1032,13 +1029,13 @@
         <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1049,16 +1046,16 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
@@ -1069,10 +1066,10 @@
         <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1083,13 +1080,13 @@
         <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1100,13 +1097,13 @@
         <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1117,13 +1114,13 @@
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1134,13 +1131,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1151,13 +1148,13 @@
         <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1168,13 +1165,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1185,13 +1182,13 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1202,13 +1199,13 @@
         <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1219,13 +1216,13 @@
         <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1236,13 +1233,13 @@
         <v>14</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1253,13 +1250,13 @@
         <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1270,13 +1267,13 @@
         <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1287,13 +1284,13 @@
         <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1304,13 +1301,13 @@
         <v>14</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1321,13 +1318,13 @@
         <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1338,16 +1335,16 @@
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1355,13 +1352,13 @@
         <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>98</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1372,13 +1369,13 @@
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1389,13 +1386,13 @@
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1406,13 +1403,13 @@
         <v>10</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1423,13 +1420,13 @@
         <v>9</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1440,13 +1437,13 @@
         <v>8</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1457,13 +1454,13 @@
         <v>10</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1474,13 +1471,13 @@
         <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1491,16 +1488,16 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -1511,13 +1508,13 @@
         <v>63</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -1525,16 +1522,16 @@
         <v>15</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
@@ -1542,16 +1539,16 @@
         <v>11</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
@@ -1559,16 +1556,16 @@
         <v>14</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
@@ -1579,13 +1576,13 @@
         <v>63</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
@@ -1596,13 +1593,13 @@
         <v>63</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
@@ -1613,13 +1610,13 @@
         <v>63</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
@@ -1630,13 +1627,13 @@
         <v>63</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>57</v>
       </c>
@@ -1647,13 +1644,13 @@
         <v>63</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -1664,13 +1661,13 @@
         <v>63</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
@@ -1681,13 +1678,13 @@
         <v>63</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>62</v>
       </c>
@@ -1698,13 +1695,13 @@
         <v>63</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -1715,10 +1712,10 @@
         <v>63</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>68</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1729,13 +1726,13 @@
         <v>3</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1746,13 +1743,13 @@
         <v>17</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1763,16 +1760,16 @@
         <v>4</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
@@ -1783,13 +1780,13 @@
         <v>63</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
@@ -1800,13 +1797,13 @@
         <v>63</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
@@ -1817,10 +1814,10 @@
         <v>63</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>68</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1831,13 +1828,13 @@
         <v>16</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>